<commit_message>
Fix composition plots and add correct ARF data
</commit_message>
<xml_diff>
--- a/VARIANCE.xlsx
+++ b/VARIANCE.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -429,7 +429,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,11 +448,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>(1/SQRT(B4^2+B5^2))^2</f>
-        <v>1.2499999999999996</v>
+        <v>0.69252077562326875</v>
       </c>
       <c r="B2" s="4">
         <f>B4^2*A2</f>
-        <v>0.19999999999999996</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>0.8</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" s="5">
         <f>SQRT(1/A2)</f>
-        <v>0.89442719099991608</v>
+        <v>1.2016655108639842</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
       </c>
       <c r="B9">
         <f>SQRT(B2)*B6</f>
-        <v>0.4</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
       </c>
       <c r="B10">
         <f>SQRT(1-B2)*B6</f>
-        <v>0.80000000000000016</v>
+        <v>1.1400000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add reference point plots, b0, bmsy, fmsy, msy boxplots
</commit_message>
<xml_diff>
--- a/VARIANCE.xlsx
+++ b/VARIANCE.xlsx
@@ -429,7 +429,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,11 +448,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>(1/SQRT(B4^2+B5^2))^2</f>
-        <v>0.69252077562326875</v>
+        <v>0.99750623441396502</v>
       </c>
       <c r="B2" s="4">
         <f>B4^2*A2</f>
-        <v>0.1</v>
+        <v>2.4937655860349131E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.38</v>
+        <v>0.05</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>1.1399999999999999</v>
+        <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" s="5">
         <f>SQRT(1/A2)</f>
-        <v>1.2016655108639842</v>
+        <v>1.0012492197250393</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
       </c>
       <c r="B9">
         <f>SQRT(B2)*B6</f>
-        <v>0.38</v>
+        <v>5.000000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
       </c>
       <c r="B10">
         <f>SQRT(1-B2)*B6</f>
-        <v>1.1400000000000001</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix gear names in selectivity plots. Some were NA
</commit_message>
<xml_diff>
--- a/VARIANCE.xlsx
+++ b/VARIANCE.xlsx
@@ -448,11 +448,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>(1/SQRT(B4^2+B5^2))^2</f>
-        <v>0.99750623441396502</v>
+        <v>1.5564202334630348</v>
       </c>
       <c r="B2" s="4">
         <f>B4^2*A2</f>
-        <v>2.4937655860349131E-3</v>
+        <v>3.8910505836575876E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" s="5">
         <f>SQRT(1/A2)</f>
-        <v>1.0012492197250393</v>
+        <v>0.80156097709406993</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
       </c>
       <c r="B9">
         <f>SQRT(B2)*B6</f>
-        <v>5.000000000000001E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
       </c>
       <c r="B10">
         <f>SQRT(1-B2)*B6</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added function to insert values or list elements into a list. Mainly for the index and selectivity comparison plots but useful for many things.
</commit_message>
<xml_diff>
--- a/VARIANCE.xlsx
+++ b/VARIANCE.xlsx
@@ -429,7 +429,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,11 +448,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>(1/SQRT(B4^2+B5^2))^2</f>
-        <v>1.5564202334630348</v>
+        <v>0.59171597633136086</v>
       </c>
       <c r="B2" s="4">
         <f>B4^2*A2</f>
-        <v>3.8910505836575876E-3</v>
+        <v>0.14792899408284022</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" s="5">
         <f>SQRT(1/A2)</f>
-        <v>0.80156097709406993</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
       </c>
       <c r="B9">
         <f>SQRT(B2)*B6</f>
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
       </c>
       <c r="B10">
         <f>SQRT(1-B2)*B6</f>
-        <v>0.8</v>
+        <v>1.2000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fix for greedy pattern matching in the comments after the paramater block in the control file and some MCMC bug fixes as well.
</commit_message>
<xml_diff>
--- a/VARIANCE.xlsx
+++ b/VARIANCE.xlsx
@@ -429,7 +429,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,11 +448,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>(1/SQRT(B4^2+B5^2))^2</f>
-        <v>0.59171597633136086</v>
+        <v>0.51546391752577314</v>
       </c>
       <c r="B2" s="4">
         <f>B4^2*A2</f>
-        <v>0.14792899408284022</v>
+        <v>0.12886597938144329</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" s="5">
         <f>SQRT(1/A2)</f>
-        <v>1.3</v>
+        <v>1.3928388277184121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
       </c>
       <c r="B10">
         <f>SQRT(1-B2)*B6</f>
-        <v>1.2000000000000002</v>
+        <v>1.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix selectivity plots for a minimum age greater than 1. Iscam always outputs selectivity from 1 to max age regardless of what the minimum age was set to.
</commit_message>
<xml_diff>
--- a/VARIANCE.xlsx
+++ b/VARIANCE.xlsx
@@ -448,11 +448,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>(1/SQRT(B4^2+B5^2))^2</f>
-        <v>0.51546391752577314</v>
+        <v>0.99009900990099031</v>
       </c>
       <c r="B2" s="4">
         <f>B4^2*A2</f>
-        <v>0.12886597938144329</v>
+        <v>9.9009900990099046E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,7 +463,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" s="5">
         <f>SQRT(1/A2)</f>
-        <v>1.3928388277184121</v>
+        <v>1.004987562112089</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -504,7 +504,7 @@
       </c>
       <c r="B9">
         <f>SQRT(B2)*B6</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
       </c>
       <c r="B10">
         <f>SQRT(1-B2)*B6</f>
-        <v>1.3</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change user message on file sourcing.
</commit_message>
<xml_diff>
--- a/VARIANCE.xlsx
+++ b/VARIANCE.xlsx
@@ -448,11 +448,11 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>(1/SQRT(B4^2+B5^2))^2</f>
-        <v>0.99009900990099031</v>
+        <v>1.5384615384615381</v>
       </c>
       <c r="B2" s="4">
         <f>B4^2*A2</f>
-        <v>9.9009900990099046E-3</v>
+        <v>1.5384615384615384E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -474,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>9</v>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" s="5">
         <f>SQRT(1/A2)</f>
-        <v>1.004987562112089</v>
+        <v>0.80622577482985502</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
       </c>
       <c r="B10">
         <f>SQRT(1-B2)*B6</f>
-        <v>0.99999999999999989</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>